<commit_message>
add daily task class
</commit_message>
<xml_diff>
--- a/Work.xlsx
+++ b/Work.xlsx
@@ -1417,7 +1417,15 @@
           <t>月曜日</t>
         </is>
       </c>
-      <c r="B2" s="5" t="n"/>
+      <c r="B2" s="5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">2022/04/01
+1. mtg (4.0h)(✔️2.0h) daily
+2. programming (2.0h)(✔️2.0h) 
+3. pc setup (1.0h)(✔️1.5h) 
+</t>
+        </is>
+      </c>
       <c r="C2" s="6" t="inlineStr">
         <is>
           <t>task</t>

</xml_diff>

<commit_message>
add excel ouput feature
</commit_message>
<xml_diff>
--- a/Work.xlsx
+++ b/Work.xlsx
@@ -1330,7 +1330,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L10"/>
+  <dimension ref="A1:O10"/>
   <sheetViews>
     <sheetView showGridLines="0" defaultGridColor="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1526,6 +1526,15 @@
       <c r="J7" s="12" t="n"/>
       <c r="K7" s="11" t="n"/>
       <c r="L7" s="13" t="n"/>
+      <c r="O7" t="inlineStr">
+        <is>
+          <t xml:space="preserve">2022/04/09
+1. ILD team weekly meeting (1.0h)(✔️2.108h) 
+2. test2 (0.0h)(✔️0.008h) 
+3. temp (0.0h)(✔️0.002h) 
+</t>
+        </is>
+      </c>
     </row>
     <row r="8" ht="13.55" customHeight="1" s="22">
       <c r="A8" s="14" t="n"/>

</xml_diff>

<commit_message>
minor change to edit info gui
</commit_message>
<xml_diff>
--- a/Work.xlsx
+++ b/Work.xlsx
@@ -62,7 +62,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -85,100 +85,13 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="11"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="8"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="8"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="11"/>
-      </right>
-      <top style="thin">
-        <color indexed="8"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="11"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="11"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="11"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="11"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="11"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="11"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="11"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1">
       <alignment vertical="bottom"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="bottom"/>
     </xf>
@@ -209,41 +122,8 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
@@ -264,7 +144,6 @@
       <rgbColor rgb="ff000000"/>
       <rgbColor rgb="ffffffff"/>
       <rgbColor rgb="ffed7d31"/>
-      <rgbColor rgb="ffaaaaaa"/>
     </indexedColors>
   </colors>
 </styleSheet>
@@ -1330,7 +1209,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O10"/>
+  <dimension ref="A1:BA8"/>
   <sheetViews>
     <sheetView showGridLines="0" defaultGridColor="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1350,10 +1229,13 @@
     <col width="189" customWidth="1" style="1" min="10" max="10"/>
     <col width="187.5" customWidth="1" style="1" min="11" max="11"/>
     <col width="136" customWidth="1" style="1" min="12" max="12"/>
-    <col width="26.5" customWidth="1" style="1" min="13" max="16384"/>
+    <col width="26.5" customWidth="1" style="1" min="13" max="14"/>
+    <col width="118" customWidth="1" style="1" min="15" max="15"/>
+    <col width="26.5" customWidth="1" style="1" min="16" max="53"/>
+    <col width="26.5" customWidth="1" style="1" min="54" max="16384"/>
   </cols>
   <sheetData>
-    <row r="1" ht="17.5" customHeight="1" s="22">
+    <row r="1" ht="17.5" customHeight="1" s="11">
       <c r="A1" s="2" t="n"/>
       <c r="B1" s="3" t="inlineStr">
         <is>
@@ -1410,27 +1292,220 @@
           <t>CW11</t>
         </is>
       </c>
+      <c r="M1" s="3" t="inlineStr">
+        <is>
+          <t>CW12</t>
+        </is>
+      </c>
+      <c r="N1" s="3" t="inlineStr">
+        <is>
+          <t>CW13</t>
+        </is>
+      </c>
+      <c r="O1" s="3" t="inlineStr">
+        <is>
+          <t>CW14</t>
+        </is>
+      </c>
+      <c r="P1" s="3" t="inlineStr">
+        <is>
+          <t>CW15</t>
+        </is>
+      </c>
+      <c r="Q1" s="3" t="inlineStr">
+        <is>
+          <t>CW16</t>
+        </is>
+      </c>
+      <c r="R1" s="3" t="inlineStr">
+        <is>
+          <t>CW17</t>
+        </is>
+      </c>
+      <c r="S1" s="3" t="inlineStr">
+        <is>
+          <t>CW18</t>
+        </is>
+      </c>
+      <c r="T1" s="3" t="inlineStr">
+        <is>
+          <t>CW19</t>
+        </is>
+      </c>
+      <c r="U1" s="3" t="inlineStr">
+        <is>
+          <t>CW20</t>
+        </is>
+      </c>
+      <c r="V1" s="3" t="inlineStr">
+        <is>
+          <t>CW21</t>
+        </is>
+      </c>
+      <c r="W1" s="3" t="inlineStr">
+        <is>
+          <t>CW22</t>
+        </is>
+      </c>
+      <c r="X1" s="3" t="inlineStr">
+        <is>
+          <t>CW23</t>
+        </is>
+      </c>
+      <c r="Y1" s="3" t="inlineStr">
+        <is>
+          <t>CW24</t>
+        </is>
+      </c>
+      <c r="Z1" s="3" t="inlineStr">
+        <is>
+          <t>CW25</t>
+        </is>
+      </c>
+      <c r="AA1" s="3" t="inlineStr">
+        <is>
+          <t>CW26</t>
+        </is>
+      </c>
+      <c r="AB1" s="3" t="inlineStr">
+        <is>
+          <t>CW27</t>
+        </is>
+      </c>
+      <c r="AC1" s="3" t="inlineStr">
+        <is>
+          <t>CW28</t>
+        </is>
+      </c>
+      <c r="AD1" s="3" t="inlineStr">
+        <is>
+          <t>CW29</t>
+        </is>
+      </c>
+      <c r="AE1" s="3" t="inlineStr">
+        <is>
+          <t>CW30</t>
+        </is>
+      </c>
+      <c r="AF1" s="3" t="inlineStr">
+        <is>
+          <t>CW31</t>
+        </is>
+      </c>
+      <c r="AG1" s="3" t="inlineStr">
+        <is>
+          <t>CW32</t>
+        </is>
+      </c>
+      <c r="AH1" s="3" t="inlineStr">
+        <is>
+          <t>CW33</t>
+        </is>
+      </c>
+      <c r="AI1" s="3" t="inlineStr">
+        <is>
+          <t>CW34</t>
+        </is>
+      </c>
+      <c r="AJ1" s="3" t="inlineStr">
+        <is>
+          <t>CW35</t>
+        </is>
+      </c>
+      <c r="AK1" s="3" t="inlineStr">
+        <is>
+          <t>CW36</t>
+        </is>
+      </c>
+      <c r="AL1" s="3" t="inlineStr">
+        <is>
+          <t>CW37</t>
+        </is>
+      </c>
+      <c r="AM1" s="3" t="inlineStr">
+        <is>
+          <t>CW38</t>
+        </is>
+      </c>
+      <c r="AN1" s="3" t="inlineStr">
+        <is>
+          <t>CW39</t>
+        </is>
+      </c>
+      <c r="AO1" s="3" t="inlineStr">
+        <is>
+          <t>CW40</t>
+        </is>
+      </c>
+      <c r="AP1" s="3" t="inlineStr">
+        <is>
+          <t>CW41</t>
+        </is>
+      </c>
+      <c r="AQ1" s="3" t="inlineStr">
+        <is>
+          <t>CW42</t>
+        </is>
+      </c>
+      <c r="AR1" s="3" t="inlineStr">
+        <is>
+          <t>CW43</t>
+        </is>
+      </c>
+      <c r="AS1" s="3" t="inlineStr">
+        <is>
+          <t>CW44</t>
+        </is>
+      </c>
+      <c r="AT1" s="3" t="inlineStr">
+        <is>
+          <t>CW45</t>
+        </is>
+      </c>
+      <c r="AU1" s="3" t="inlineStr">
+        <is>
+          <t>CW46</t>
+        </is>
+      </c>
+      <c r="AV1" s="3" t="inlineStr">
+        <is>
+          <t>CW47</t>
+        </is>
+      </c>
+      <c r="AW1" s="3" t="inlineStr">
+        <is>
+          <t>CW48</t>
+        </is>
+      </c>
+      <c r="AX1" s="3" t="inlineStr">
+        <is>
+          <t>CW49</t>
+        </is>
+      </c>
+      <c r="AY1" s="3" t="inlineStr">
+        <is>
+          <t>CW50</t>
+        </is>
+      </c>
+      <c r="AZ1" s="3" t="inlineStr">
+        <is>
+          <t>CW51</t>
+        </is>
+      </c>
+      <c r="BA1" s="3" t="inlineStr">
+        <is>
+          <t>CW52</t>
+        </is>
+      </c>
     </row>
-    <row r="2" ht="95" customHeight="1" s="22">
+    <row r="2" ht="95" customHeight="1" s="11">
       <c r="A2" s="4" t="inlineStr">
         <is>
           <t>月曜日</t>
         </is>
       </c>
-      <c r="B2" s="5" t="inlineStr">
-        <is>
-          <t xml:space="preserve">2022/04/01
-1. MTG (4.0h)(✔️2.0h) daily
-2. python programming (2.0h)(✔️2.0h) 
-3. pc setup (1.0h)(✔️1.5h) 
-</t>
-        </is>
-      </c>
-      <c r="C2" s="6" t="inlineStr">
-        <is>
-          <t>task</t>
-        </is>
-      </c>
+      <c r="B2" s="5" t="n"/>
+      <c r="C2" s="6" t="n"/>
       <c r="D2" s="7" t="n"/>
       <c r="E2" s="7" t="n"/>
       <c r="F2" s="8" t="n"/>
@@ -1440,8 +1515,49 @@
       <c r="J2" s="8" t="n"/>
       <c r="K2" s="7" t="n"/>
       <c r="L2" s="9" t="n"/>
+      <c r="M2" s="2" t="n"/>
+      <c r="N2" s="2" t="n"/>
+      <c r="O2" s="2" t="n"/>
+      <c r="P2" s="2" t="n"/>
+      <c r="Q2" s="2" t="n"/>
+      <c r="R2" s="2" t="n"/>
+      <c r="S2" s="2" t="n"/>
+      <c r="T2" s="2" t="n"/>
+      <c r="U2" s="2" t="n"/>
+      <c r="V2" s="2" t="n"/>
+      <c r="W2" s="2" t="n"/>
+      <c r="X2" s="2" t="n"/>
+      <c r="Y2" s="2" t="n"/>
+      <c r="Z2" s="2" t="n"/>
+      <c r="AA2" s="2" t="n"/>
+      <c r="AB2" s="2" t="n"/>
+      <c r="AC2" s="2" t="n"/>
+      <c r="AD2" s="2" t="n"/>
+      <c r="AE2" s="2" t="n"/>
+      <c r="AF2" s="2" t="n"/>
+      <c r="AG2" s="2" t="n"/>
+      <c r="AH2" s="2" t="n"/>
+      <c r="AI2" s="2" t="n"/>
+      <c r="AJ2" s="2" t="n"/>
+      <c r="AK2" s="2" t="n"/>
+      <c r="AL2" s="2" t="n"/>
+      <c r="AM2" s="2" t="n"/>
+      <c r="AN2" s="2" t="n"/>
+      <c r="AO2" s="2" t="n"/>
+      <c r="AP2" s="2" t="n"/>
+      <c r="AQ2" s="2" t="n"/>
+      <c r="AR2" s="2" t="n"/>
+      <c r="AS2" s="2" t="n"/>
+      <c r="AT2" s="2" t="n"/>
+      <c r="AU2" s="2" t="n"/>
+      <c r="AV2" s="2" t="n"/>
+      <c r="AW2" s="2" t="n"/>
+      <c r="AX2" s="2" t="n"/>
+      <c r="AY2" s="2" t="n"/>
+      <c r="AZ2" s="2" t="n"/>
+      <c r="BA2" s="2" t="n"/>
     </row>
-    <row r="3" ht="133" customHeight="1" s="22">
+    <row r="3" ht="133" customHeight="1" s="11">
       <c r="A3" s="4" t="inlineStr">
         <is>
           <t>火曜日</t>
@@ -1458,8 +1574,49 @@
       <c r="J3" s="8" t="n"/>
       <c r="K3" s="7" t="n"/>
       <c r="L3" s="9" t="n"/>
+      <c r="M3" s="2" t="n"/>
+      <c r="N3" s="2" t="n"/>
+      <c r="O3" s="2" t="n"/>
+      <c r="P3" s="2" t="n"/>
+      <c r="Q3" s="2" t="n"/>
+      <c r="R3" s="2" t="n"/>
+      <c r="S3" s="2" t="n"/>
+      <c r="T3" s="2" t="n"/>
+      <c r="U3" s="2" t="n"/>
+      <c r="V3" s="2" t="n"/>
+      <c r="W3" s="2" t="n"/>
+      <c r="X3" s="2" t="n"/>
+      <c r="Y3" s="2" t="n"/>
+      <c r="Z3" s="2" t="n"/>
+      <c r="AA3" s="2" t="n"/>
+      <c r="AB3" s="2" t="n"/>
+      <c r="AC3" s="2" t="n"/>
+      <c r="AD3" s="2" t="n"/>
+      <c r="AE3" s="2" t="n"/>
+      <c r="AF3" s="2" t="n"/>
+      <c r="AG3" s="2" t="n"/>
+      <c r="AH3" s="2" t="n"/>
+      <c r="AI3" s="2" t="n"/>
+      <c r="AJ3" s="2" t="n"/>
+      <c r="AK3" s="2" t="n"/>
+      <c r="AL3" s="2" t="n"/>
+      <c r="AM3" s="2" t="n"/>
+      <c r="AN3" s="2" t="n"/>
+      <c r="AO3" s="2" t="n"/>
+      <c r="AP3" s="2" t="n"/>
+      <c r="AQ3" s="2" t="n"/>
+      <c r="AR3" s="2" t="n"/>
+      <c r="AS3" s="2" t="n"/>
+      <c r="AT3" s="2" t="n"/>
+      <c r="AU3" s="2" t="n"/>
+      <c r="AV3" s="2" t="n"/>
+      <c r="AW3" s="2" t="n"/>
+      <c r="AX3" s="2" t="n"/>
+      <c r="AY3" s="2" t="n"/>
+      <c r="AZ3" s="2" t="n"/>
+      <c r="BA3" s="2" t="n"/>
     </row>
-    <row r="4" ht="76" customHeight="1" s="22">
+    <row r="4" ht="76" customHeight="1" s="11">
       <c r="A4" s="4" t="inlineStr">
         <is>
           <t>水曜日</t>
@@ -1476,8 +1633,49 @@
       <c r="J4" s="8" t="n"/>
       <c r="K4" s="7" t="n"/>
       <c r="L4" s="9" t="n"/>
+      <c r="M4" s="2" t="n"/>
+      <c r="N4" s="2" t="n"/>
+      <c r="O4" s="2" t="n"/>
+      <c r="P4" s="2" t="n"/>
+      <c r="Q4" s="2" t="n"/>
+      <c r="R4" s="2" t="n"/>
+      <c r="S4" s="2" t="n"/>
+      <c r="T4" s="2" t="n"/>
+      <c r="U4" s="2" t="n"/>
+      <c r="V4" s="2" t="n"/>
+      <c r="W4" s="2" t="n"/>
+      <c r="X4" s="2" t="n"/>
+      <c r="Y4" s="2" t="n"/>
+      <c r="Z4" s="2" t="n"/>
+      <c r="AA4" s="2" t="n"/>
+      <c r="AB4" s="2" t="n"/>
+      <c r="AC4" s="2" t="n"/>
+      <c r="AD4" s="2" t="n"/>
+      <c r="AE4" s="2" t="n"/>
+      <c r="AF4" s="2" t="n"/>
+      <c r="AG4" s="2" t="n"/>
+      <c r="AH4" s="2" t="n"/>
+      <c r="AI4" s="2" t="n"/>
+      <c r="AJ4" s="2" t="n"/>
+      <c r="AK4" s="2" t="n"/>
+      <c r="AL4" s="2" t="n"/>
+      <c r="AM4" s="2" t="n"/>
+      <c r="AN4" s="2" t="n"/>
+      <c r="AO4" s="2" t="n"/>
+      <c r="AP4" s="2" t="n"/>
+      <c r="AQ4" s="2" t="n"/>
+      <c r="AR4" s="2" t="n"/>
+      <c r="AS4" s="2" t="n"/>
+      <c r="AT4" s="2" t="n"/>
+      <c r="AU4" s="2" t="n"/>
+      <c r="AV4" s="2" t="n"/>
+      <c r="AW4" s="2" t="n"/>
+      <c r="AX4" s="2" t="n"/>
+      <c r="AY4" s="2" t="n"/>
+      <c r="AZ4" s="2" t="n"/>
+      <c r="BA4" s="2" t="n"/>
     </row>
-    <row r="5" ht="76" customHeight="1" s="22">
+    <row r="5" ht="76" customHeight="1" s="11">
       <c r="A5" s="4" t="inlineStr">
         <is>
           <t>木曜日</t>
@@ -1494,8 +1692,49 @@
       <c r="J5" s="8" t="n"/>
       <c r="K5" s="7" t="n"/>
       <c r="L5" s="9" t="n"/>
+      <c r="M5" s="2" t="n"/>
+      <c r="N5" s="2" t="n"/>
+      <c r="O5" s="2" t="n"/>
+      <c r="P5" s="2" t="n"/>
+      <c r="Q5" s="2" t="n"/>
+      <c r="R5" s="2" t="n"/>
+      <c r="S5" s="2" t="n"/>
+      <c r="T5" s="2" t="n"/>
+      <c r="U5" s="2" t="n"/>
+      <c r="V5" s="2" t="n"/>
+      <c r="W5" s="2" t="n"/>
+      <c r="X5" s="2" t="n"/>
+      <c r="Y5" s="2" t="n"/>
+      <c r="Z5" s="2" t="n"/>
+      <c r="AA5" s="2" t="n"/>
+      <c r="AB5" s="2" t="n"/>
+      <c r="AC5" s="2" t="n"/>
+      <c r="AD5" s="2" t="n"/>
+      <c r="AE5" s="2" t="n"/>
+      <c r="AF5" s="2" t="n"/>
+      <c r="AG5" s="2" t="n"/>
+      <c r="AH5" s="2" t="n"/>
+      <c r="AI5" s="2" t="n"/>
+      <c r="AJ5" s="2" t="n"/>
+      <c r="AK5" s="2" t="n"/>
+      <c r="AL5" s="2" t="n"/>
+      <c r="AM5" s="2" t="n"/>
+      <c r="AN5" s="2" t="n"/>
+      <c r="AO5" s="2" t="n"/>
+      <c r="AP5" s="2" t="n"/>
+      <c r="AQ5" s="2" t="n"/>
+      <c r="AR5" s="2" t="n"/>
+      <c r="AS5" s="2" t="n"/>
+      <c r="AT5" s="2" t="n"/>
+      <c r="AU5" s="2" t="n"/>
+      <c r="AV5" s="2" t="n"/>
+      <c r="AW5" s="2" t="n"/>
+      <c r="AX5" s="2" t="n"/>
+      <c r="AY5" s="2" t="n"/>
+      <c r="AZ5" s="2" t="n"/>
+      <c r="BA5" s="2" t="n"/>
     </row>
-    <row r="6" ht="76" customHeight="1" s="22">
+    <row r="6" ht="76" customHeight="1" s="11">
       <c r="A6" s="4" t="inlineStr">
         <is>
           <t>金曜日</t>
@@ -1512,71 +1751,182 @@
       <c r="J6" s="8" t="n"/>
       <c r="K6" s="7" t="n"/>
       <c r="L6" s="9" t="n"/>
+      <c r="M6" s="2" t="n"/>
+      <c r="N6" s="2" t="n"/>
+      <c r="O6" s="2" t="n"/>
+      <c r="P6" s="2" t="n"/>
+      <c r="Q6" s="2" t="n"/>
+      <c r="R6" s="2" t="n"/>
+      <c r="S6" s="2" t="n"/>
+      <c r="T6" s="2" t="n"/>
+      <c r="U6" s="2" t="n"/>
+      <c r="V6" s="2" t="n"/>
+      <c r="W6" s="2" t="n"/>
+      <c r="X6" s="2" t="n"/>
+      <c r="Y6" s="2" t="n"/>
+      <c r="Z6" s="2" t="n"/>
+      <c r="AA6" s="2" t="n"/>
+      <c r="AB6" s="2" t="n"/>
+      <c r="AC6" s="2" t="n"/>
+      <c r="AD6" s="2" t="n"/>
+      <c r="AE6" s="2" t="n"/>
+      <c r="AF6" s="2" t="n"/>
+      <c r="AG6" s="2" t="n"/>
+      <c r="AH6" s="2" t="n"/>
+      <c r="AI6" s="2" t="n"/>
+      <c r="AJ6" s="2" t="n"/>
+      <c r="AK6" s="2" t="n"/>
+      <c r="AL6" s="2" t="n"/>
+      <c r="AM6" s="2" t="n"/>
+      <c r="AN6" s="2" t="n"/>
+      <c r="AO6" s="2" t="n"/>
+      <c r="AP6" s="2" t="n"/>
+      <c r="AQ6" s="2" t="n"/>
+      <c r="AR6" s="2" t="n"/>
+      <c r="AS6" s="2" t="n"/>
+      <c r="AT6" s="2" t="n"/>
+      <c r="AU6" s="2" t="n"/>
+      <c r="AV6" s="2" t="n"/>
+      <c r="AW6" s="2" t="n"/>
+      <c r="AX6" s="2" t="n"/>
+      <c r="AY6" s="2" t="n"/>
+      <c r="AZ6" s="2" t="n"/>
+      <c r="BA6" s="2" t="n"/>
     </row>
-    <row r="7" ht="13.55" customHeight="1" s="22">
-      <c r="A7" s="10" t="n"/>
-      <c r="B7" s="11" t="n"/>
-      <c r="C7" s="11" t="n"/>
-      <c r="D7" s="11" t="n"/>
-      <c r="E7" s="11" t="n"/>
-      <c r="F7" s="12" t="n"/>
-      <c r="G7" s="11" t="n"/>
-      <c r="H7" s="11" t="n"/>
-      <c r="I7" s="11" t="n"/>
-      <c r="J7" s="12" t="n"/>
-      <c r="K7" s="11" t="n"/>
-      <c r="L7" s="13" t="n"/>
-      <c r="O7" t="inlineStr">
+    <row r="7" ht="55.65" customHeight="1" s="11">
+      <c r="A7" s="4" t="inlineStr">
+        <is>
+          <t>土曜日</t>
+        </is>
+      </c>
+      <c r="B7" s="2" t="n"/>
+      <c r="C7" s="2" t="n"/>
+      <c r="D7" s="2" t="n"/>
+      <c r="E7" s="2" t="n"/>
+      <c r="F7" s="10" t="n"/>
+      <c r="G7" s="2" t="n"/>
+      <c r="H7" s="2" t="n"/>
+      <c r="I7" s="2" t="n"/>
+      <c r="J7" s="10" t="n"/>
+      <c r="K7" s="2" t="n"/>
+      <c r="L7" s="2" t="n"/>
+      <c r="M7" s="2" t="n"/>
+      <c r="N7" s="2" t="n"/>
+      <c r="O7" s="2" t="inlineStr">
         <is>
           <t xml:space="preserve">2022/04/09
 1. ILD team weekly meeting (1.0h)(✔️2.108h) 
 2. test2 (0.0h)(✔️0.008h) 
 3. temp (0.0h)(✔️0.002h) 
+1. ILD team weekly meeting (1.0h)(✔️2.108h) 
+2. test2 (0.0h)(✔️0.008h) 
+3. temp (0.0h)(✔️0.002h) 
+1. ILD team weekly meeting (1.0h)(✔️2.108h) 
+2. test2 (0.0h)(✔️0.008h) 
+3. temp (0.0h)(✔️0.002h) 
+1. ILD team weekly meeting (1.0h)(✔️2.11h) 
+2. test2 (0.0h)(✔️0.009h) 
+3. temp (0.0h)(✔️0.003h) 
 </t>
         </is>
       </c>
+      <c r="P7" s="2" t="n"/>
+      <c r="Q7" s="2" t="n"/>
+      <c r="R7" s="2" t="n"/>
+      <c r="S7" s="2" t="n"/>
+      <c r="T7" s="2" t="n"/>
+      <c r="U7" s="2" t="n"/>
+      <c r="V7" s="2" t="n"/>
+      <c r="W7" s="2" t="n"/>
+      <c r="X7" s="2" t="n"/>
+      <c r="Y7" s="2" t="n"/>
+      <c r="Z7" s="2" t="n"/>
+      <c r="AA7" s="2" t="n"/>
+      <c r="AB7" s="2" t="n"/>
+      <c r="AC7" s="2" t="n"/>
+      <c r="AD7" s="2" t="n"/>
+      <c r="AE7" s="2" t="n"/>
+      <c r="AF7" s="2" t="n"/>
+      <c r="AG7" s="2" t="n"/>
+      <c r="AH7" s="2" t="n"/>
+      <c r="AI7" s="2" t="n"/>
+      <c r="AJ7" s="2" t="n"/>
+      <c r="AK7" s="2" t="n"/>
+      <c r="AL7" s="2" t="n"/>
+      <c r="AM7" s="2" t="n"/>
+      <c r="AN7" s="2" t="n"/>
+      <c r="AO7" s="2" t="n"/>
+      <c r="AP7" s="2" t="n"/>
+      <c r="AQ7" s="2" t="n"/>
+      <c r="AR7" s="2" t="n"/>
+      <c r="AS7" s="2" t="n"/>
+      <c r="AT7" s="2" t="n"/>
+      <c r="AU7" s="2" t="n"/>
+      <c r="AV7" s="2" t="n"/>
+      <c r="AW7" s="2" t="n"/>
+      <c r="AX7" s="2" t="n"/>
+      <c r="AY7" s="2" t="n"/>
+      <c r="AZ7" s="2" t="n"/>
+      <c r="BA7" s="2" t="n"/>
     </row>
-    <row r="8" ht="13.55" customHeight="1" s="22">
-      <c r="A8" s="14" t="n"/>
-      <c r="B8" s="15" t="n"/>
-      <c r="C8" s="15" t="n"/>
-      <c r="D8" s="15" t="n"/>
-      <c r="E8" s="15" t="n"/>
-      <c r="F8" s="16" t="n"/>
-      <c r="G8" s="15" t="n"/>
-      <c r="H8" s="15" t="n"/>
-      <c r="I8" s="15" t="n"/>
-      <c r="J8" s="16" t="n"/>
-      <c r="K8" s="15" t="n"/>
-      <c r="L8" s="17" t="n"/>
-    </row>
-    <row r="9" ht="13.55" customHeight="1" s="22">
-      <c r="A9" s="14" t="n"/>
-      <c r="B9" s="15" t="n"/>
-      <c r="C9" s="15" t="n"/>
-      <c r="D9" s="15" t="n"/>
-      <c r="E9" s="15" t="n"/>
-      <c r="F9" s="16" t="n"/>
-      <c r="G9" s="15" t="n"/>
-      <c r="H9" s="15" t="n"/>
-      <c r="I9" s="15" t="n"/>
-      <c r="J9" s="16" t="n"/>
-      <c r="K9" s="15" t="n"/>
-      <c r="L9" s="17" t="n"/>
-    </row>
-    <row r="10" ht="13.55" customHeight="1" s="22">
-      <c r="A10" s="18" t="n"/>
-      <c r="B10" s="19" t="n"/>
-      <c r="C10" s="19" t="n"/>
-      <c r="D10" s="19" t="n"/>
-      <c r="E10" s="19" t="n"/>
-      <c r="F10" s="20" t="n"/>
-      <c r="G10" s="19" t="n"/>
-      <c r="H10" s="19" t="n"/>
-      <c r="I10" s="19" t="n"/>
-      <c r="J10" s="20" t="n"/>
-      <c r="K10" s="19" t="n"/>
-      <c r="L10" s="21" t="n"/>
+    <row r="8" ht="62.1" customHeight="1" s="11">
+      <c r="A8" s="4" t="inlineStr">
+        <is>
+          <t>日曜日</t>
+        </is>
+      </c>
+      <c r="B8" s="2" t="n"/>
+      <c r="C8" s="2" t="n"/>
+      <c r="D8" s="2" t="n"/>
+      <c r="E8" s="2" t="n"/>
+      <c r="F8" s="10" t="n"/>
+      <c r="G8" s="2" t="n"/>
+      <c r="H8" s="2" t="n"/>
+      <c r="I8" s="2" t="n"/>
+      <c r="J8" s="10" t="n"/>
+      <c r="K8" s="2" t="n"/>
+      <c r="L8" s="2" t="n"/>
+      <c r="M8" s="2" t="n"/>
+      <c r="N8" s="2" t="n"/>
+      <c r="O8" s="2" t="n"/>
+      <c r="P8" s="2" t="n"/>
+      <c r="Q8" s="2" t="n"/>
+      <c r="R8" s="2" t="n"/>
+      <c r="S8" s="2" t="n"/>
+      <c r="T8" s="2" t="n"/>
+      <c r="U8" s="2" t="n"/>
+      <c r="V8" s="2" t="n"/>
+      <c r="W8" s="2" t="n"/>
+      <c r="X8" s="2" t="n"/>
+      <c r="Y8" s="2" t="n"/>
+      <c r="Z8" s="2" t="n"/>
+      <c r="AA8" s="2" t="n"/>
+      <c r="AB8" s="2" t="n"/>
+      <c r="AC8" s="2" t="n"/>
+      <c r="AD8" s="2" t="n"/>
+      <c r="AE8" s="2" t="n"/>
+      <c r="AF8" s="2" t="n"/>
+      <c r="AG8" s="2" t="n"/>
+      <c r="AH8" s="2" t="n"/>
+      <c r="AI8" s="2" t="n"/>
+      <c r="AJ8" s="2" t="n"/>
+      <c r="AK8" s="2" t="n"/>
+      <c r="AL8" s="2" t="n"/>
+      <c r="AM8" s="2" t="n"/>
+      <c r="AN8" s="2" t="n"/>
+      <c r="AO8" s="2" t="n"/>
+      <c r="AP8" s="2" t="n"/>
+      <c r="AQ8" s="2" t="n"/>
+      <c r="AR8" s="2" t="n"/>
+      <c r="AS8" s="2" t="n"/>
+      <c r="AT8" s="2" t="n"/>
+      <c r="AU8" s="2" t="n"/>
+      <c r="AV8" s="2" t="n"/>
+      <c r="AW8" s="2" t="n"/>
+      <c r="AX8" s="2" t="n"/>
+      <c r="AY8" s="2" t="n"/>
+      <c r="AZ8" s="2" t="n"/>
+      <c r="BA8" s="2" t="n"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>